<commit_message>
Adding new results for ram_access_time
stubbing old results
fixes to makefile
</commit_message>
<xml_diff>
--- a/operations/2_memory/ram_access_time/logs/ram_access_time.xlsx
+++ b/operations/2_memory/ram_access_time/logs/ram_access_time.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohitgupta/Desktop/UCSD/quarter_4/cse_221/project/CSE221_project/operations/2_memory/ram_access_time/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75ADD9D-9EF0-C645-BDC4-1461CDC2FC63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{739FF09F-F932-334A-98CF-25253BD067CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="ram_access_time" sheetId="1" r:id="rId1"/>
@@ -28,18 +28,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Log2 (memory sizes in bytes)</t>
+    <t>median cycles</t>
   </si>
   <si>
-    <t>Memory access times (clock cycles)</t>
+    <t>average cycles</t>
+  </si>
+  <si>
+    <t>log(average cycles)</t>
+  </si>
+  <si>
+    <t>memory size</t>
+  </si>
+  <si>
+    <t>log(memory size)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -613,7 +622,29 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Memory access times (clock cycles)</a:t>
+              <a:t>log2</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>(Access Time in cycles) </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>VS</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>log2(Memory Size Accessed in bytes)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -656,17 +687,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ram_access_time!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Memory access times (clock cycles)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -693,10 +713,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ram_access_time!$B$2:$B$77</c:f>
+              <c:f>ram_access_time!$B$2:$B$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="76"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -704,463 +724,421 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.5849625</c:v>
+                  <c:v>11.584962500721158</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.32192809</c:v>
+                  <c:v>12.321928094887364</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.5849625</c:v>
+                  <c:v>12.584962500721158</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.80735492</c:v>
+                  <c:v>12.807354922057604</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.169924999999999</c:v>
+                  <c:v>13.169925001442312</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.32192809</c:v>
+                  <c:v>13.321928094887364</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.45943162</c:v>
+                  <c:v>13.459431618637296</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.5849625</c:v>
+                  <c:v>13.584962500721158</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.70043972</c:v>
+                  <c:v>13.700439718141093</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.80735492</c:v>
+                  <c:v>13.807354922057604</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13.906890600000001</c:v>
+                  <c:v>13.906890595608518</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.087462840000001</c:v>
+                  <c:v>14.087462841250341</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.169924999999999</c:v>
+                  <c:v>14.169925001442312</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.24792751</c:v>
+                  <c:v>14.247927513443587</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14.32192809</c:v>
+                  <c:v>14.321928094887364</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14.392317419999999</c:v>
+                  <c:v>14.392317422778762</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14.45943162</c:v>
+                  <c:v>14.459431618637296</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>14.52356196</c:v>
+                  <c:v>14.523561956057014</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14.5849625</c:v>
+                  <c:v>14.584962500721158</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>14.643856189999999</c:v>
+                  <c:v>14.643856189774723</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14.70043972</c:v>
+                  <c:v>14.700439718141093</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>14.754887500000001</c:v>
+                  <c:v>14.754887502163468</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>14.80735492</c:v>
+                  <c:v>14.807354922057604</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14.857981000000001</c:v>
+                  <c:v>14.857980995127573</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14.906890600000001</c:v>
+                  <c:v>14.906890595608518</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>14.95419631</c:v>
+                  <c:v>14.954196310386875</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>15.04439412</c:v>
+                  <c:v>15.584962500721158</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>15.087462840000001</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>15.129283020000001</c:v>
+                  <c:v>16.321928094887365</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>15.169924999999999</c:v>
+                  <c:v>16.584962500721158</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>15.20945337</c:v>
+                  <c:v>16.807354922057606</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>15.24792751</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>15.28540222</c:v>
+                  <c:v>17.584962500721158</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>15.32192809</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>15.357552</c:v>
+                  <c:v>18.321928094887365</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>15.392317419999999</c:v>
+                  <c:v>18.584962500721154</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>15.42626475</c:v>
+                  <c:v>18.807354922057606</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>15.45943162</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>15.5849625</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>16.32192809</c:v>
+                  <c:v>21.584962500721154</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>16.5849625</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>16.807354920000002</c:v>
+                  <c:v>22.321928094887362</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>17</c:v>
+                  <c:v>22.584962500721158</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>17.169924999999999</c:v>
+                  <c:v>22.807354922057606</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>17.32192809</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>17.45943162</c:v>
+                  <c:v>23.169925001442316</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>17.5849625</c:v>
+                  <c:v>23.321928094887362</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>17.700439719999999</c:v>
+                  <c:v>23.459431618637296</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>17.807354920000002</c:v>
+                  <c:v>23.584962500721158</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>17.906890600000001</c:v>
+                  <c:v>23.700439718141094</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>18</c:v>
+                  <c:v>23.807354922057602</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>18.087462840000001</c:v>
+                  <c:v>23.906890595608516</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>18.169924999999999</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>18.24792751</c:v>
+                  <c:v>24.087462841250343</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>18.32192809</c:v>
+                  <c:v>24.169925001442312</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>18.392317420000001</c:v>
+                  <c:v>24.247927513443585</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>18.45943162</c:v>
+                  <c:v>24.321928094887365</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>18.523561959999999</c:v>
+                  <c:v>24.392317422778763</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>18.5849625</c:v>
+                  <c:v>24.459431618637296</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>18.643856190000001</c:v>
+                  <c:v>24.523561956057016</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>18.700439719999999</c:v>
+                  <c:v>24.584962500721158</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>18.754887499999999</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>18.807354920000002</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>18.857980999999999</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>18.906890600000001</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>18.95419631</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>21</c:v>
+                  <c:v>24.643856189774727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ram_access_time!$C$2:$C$77</c:f>
+              <c:f>ram_access_time!$C$2:$C$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="76"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1.4594316186372973</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1.3219280948873624</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9200000000000017</c:v>
+                  <c:v>1.1176950426697545</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8800000000000026</c:v>
+                  <c:v>1.207892851641333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9500000000000028</c:v>
+                  <c:v>0.67807190511263782</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2100000000000009</c:v>
+                  <c:v>1.028569152196771</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9299999999999997</c:v>
+                  <c:v>1.028569152196771</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9699999999999989</c:v>
+                  <c:v>1.0214797274104515</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0600000000000023</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1499999999999986</c:v>
+                  <c:v>0.98550043030488488</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.2700000000000031</c:v>
+                  <c:v>0.97085365434048343</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.2899999999999991</c:v>
+                  <c:v>1.0143552929770701</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1199999999999974</c:v>
+                  <c:v>1.0772429989324603</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1000000000000014</c:v>
+                  <c:v>1.0496307677246004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.2299999999999969</c:v>
+                  <c:v>1.0840642647884746</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1599999999999966</c:v>
+                  <c:v>0.97819562968165163</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.2199999999999989</c:v>
+                  <c:v>0.94860084749335571</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.009999999999998</c:v>
+                  <c:v>0.90303827011291216</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.2100000000000009</c:v>
+                  <c:v>0.95605665241240301</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.0200000000000031</c:v>
+                  <c:v>1.2203299548795556</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.9500000000000028</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1000000000000014</c:v>
+                  <c:v>1.0214797274104515</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2</c:v>
+                  <c:v>0.97819562968165163</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.8999999999999986</c:v>
+                  <c:v>1.0565835283663676</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.0499999999999972</c:v>
+                  <c:v>1.1243281350022019</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.1199999999999974</c:v>
+                  <c:v>1.2630344058337937</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.2100000000000009</c:v>
+                  <c:v>1.1440463696167069</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.2700000000000031</c:v>
+                  <c:v>1.2203299548795556</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3999999999999986</c:v>
+                  <c:v>1.3785116232537298</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.5600000000000023</c:v>
+                  <c:v>1.7004397181410922</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0799999999999983</c:v>
+                  <c:v>2.6064422281316078</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5.6499999999999986</c:v>
+                  <c:v>2.3074285251922473</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.5300000000000011</c:v>
+                  <c:v>2.304511041809953</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.9099999999999966</c:v>
+                  <c:v>1.9963887464476213</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.25</c:v>
+                  <c:v>2.2986583155645151</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.0600000000000023</c:v>
+                  <c:v>2.4302852729777809</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.5499999999999972</c:v>
+                  <c:v>5.6458745503090304</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.3999999999999986</c:v>
+                  <c:v>3.1667154449664223</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.7199999999999989</c:v>
+                  <c:v>4.0098845889318442</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.6899999999999977</c:v>
+                  <c:v>4.4685833170068276</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.8599999999999994</c:v>
+                  <c:v>4.4899282194051828</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.0499999999999972</c:v>
+                  <c:v>4.6229303509201767</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.7199999999999989</c:v>
+                  <c:v>4.7554217347342425</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.9799999999999969</c:v>
+                  <c:v>7.0296737346264209</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.8599999999999994</c:v>
+                  <c:v>8.0635029423061582</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.0300000000000011</c:v>
+                  <c:v>6.9971794809376213</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>71.77</c:v>
+                  <c:v>7.5055734002820182</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6.9099999999999966</c:v>
+                  <c:v>7.6603525096709211</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.0399999999999991</c:v>
+                  <c:v>8.3048760500448893</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5.93</c:v>
+                  <c:v>9.179088012680273</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>9.4799999999999969</c:v>
+                  <c:v>7.8182626083044742</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>7.8800000000000026</c:v>
+                  <c:v>7.8026456041288244</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>6.5200000000000031</c:v>
+                  <c:v>7.7631459581494759</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>8.7100000000000009</c:v>
+                  <c:v>7.8880125854028291</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>19.310000000000002</c:v>
+                  <c:v>7.768184324776926</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>18.009999999999998</c:v>
+                  <c:v>7.7666614118172621</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>16.659999999999997</c:v>
+                  <c:v>8.0164183174068757</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>16.759999999999998</c:v>
+                  <c:v>7.7781428544637716</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>15</c:v>
+                  <c:v>8.0241977648948684</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>22.619999999999997</c:v>
+                  <c:v>7.8578566195043322</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>89.36</c:v>
+                  <c:v>7.8548683832602366</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>21.840000000000003</c:v>
+                  <c:v>8.0350739973776228</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>22.42</c:v>
+                  <c:v>8.2035437752826574</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>23.67</c:v>
+                  <c:v>7.898389766534847</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>24.93</c:v>
+                  <c:v>7.9302050977844338</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>22.689999999999998</c:v>
+                  <c:v>8.2011437320530334</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>37.480000000000004</c:v>
+                  <c:v>7.9467893339488453</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>23.32</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>24.880000000000003</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>119.68</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>26.14</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>93.72</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>26.71</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>44.08</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>183.84</c:v>
+                  <c:v>7.8644337963656232</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1187,7 +1165,769 @@
         <c:axId val="174108672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="21"/>
+          <c:max val="25"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="117135024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="117135024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="174108672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Access Time in cycles</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>VS</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>log2(Memory Size Accessed in bytes)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ram_access_time!$B$2:$B$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="69"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.321928094887364</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.807354922057604</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.169925001442312</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.321928094887364</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.459431618637296</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.700439718141093</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.807354922057604</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.906890595608518</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.087462841250341</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14.169925001442312</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.247927513443587</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.321928094887364</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.392317422778762</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14.459431618637296</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14.523561956057014</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14.643856189774723</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14.700439718141093</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14.754887502163468</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.807354922057604</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.857980995127573</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.906890595608518</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.954196310386875</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16.321928094887365</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>16.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>16.807354922057606</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>18.321928094887365</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>18.584962500721154</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>18.807354922057606</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>21.584962500721154</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>22.321928094887362</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>22.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>22.807354922057606</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>23.169925001442316</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>23.321928094887362</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>23.459431618637296</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>23.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>23.700439718141094</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>23.807354922057602</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>23.906890595608516</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>24.087462841250343</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>24.169925001442312</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>24.247927513443585</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>24.321928094887365</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>24.392317422778763</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>24.459431618637296</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>24.523561956057016</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>24.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>24.643856189774727</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ram_access_time!$D$2:$D$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="69"/>
+                <c:pt idx="0">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.97</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.87</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.97</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.21</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.09</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.95</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.9400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.99</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.92</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.39</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>50.07</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.98</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>16.11</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>22.14</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>22.47</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>24.64</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>27.01</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>130.66</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>267.52</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>127.75</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>181.72</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>202.3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>316.24</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>579.66999999999996</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>225.7</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>223.27</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>217.24</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>236.88</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>217.77</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>258.93</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>219.51</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>260.33</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>231.98</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>231.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>262.3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>294.79000000000002</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>238.59</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>243.91</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>294.3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>246.73</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>233.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E7DC-DD44-8AE2-4D696E619C33}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="174108672"/>
+        <c:axId val="117135024"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="174108672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="26"/>
           <c:min val="10"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1309,7 +2049,7 @@
         <c:crossAx val="174108672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
+        <c:majorUnit val="25"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1397,6 +2137,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1913,27 +2693,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>643165</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>137</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>226785</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B164C10-A0F2-294F-A6BB-83FD31A1610D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21800C3D-C44E-5E48-A01C-768E8A3EF002}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1946,6 +3242,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>398236</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>53522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>657679</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55CDF678-B187-B64C-BFD9-ACA1B6EAB1DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2535,1627 +3867,1633 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride2.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D108"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="56" workbookViewId="0">
+      <selection activeCell="Q73" sqref="Q73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1024</v>
       </c>
       <c r="B2">
+        <f>LOG(A2,2)</f>
         <v>10</v>
       </c>
       <c r="C2">
-        <f>D2-32</f>
-        <v>2</v>
+        <f>LOG(D2,2)</f>
+        <v>1.4594316186372973</v>
       </c>
       <c r="D2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.75</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2048</v>
       </c>
       <c r="B3">
+        <f t="shared" ref="B3:B66" si="0">LOG(A3,2)</f>
         <v>11</v>
       </c>
       <c r="C3">
-        <f>D3-32</f>
-        <v>2</v>
+        <f t="shared" ref="C3:C66" si="1">LOG(D3,2)</f>
+        <v>1.3219280948873624</v>
       </c>
       <c r="D3">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.5</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3072</v>
       </c>
       <c r="B4">
-        <v>11.5849625</v>
+        <f t="shared" si="0"/>
+        <v>11.584962500721158</v>
       </c>
       <c r="C4">
-        <f>D4-32</f>
-        <v>1.9200000000000017</v>
+        <f t="shared" si="1"/>
+        <v>1.1176950426697545</v>
       </c>
       <c r="D4">
-        <v>33.92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.17</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4096</v>
       </c>
       <c r="B5">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C68" si="0">D5-32</f>
-        <v>1.8800000000000026</v>
+        <f t="shared" si="1"/>
+        <v>1.207892851641333</v>
       </c>
       <c r="D5">
-        <v>33.880000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.31</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5120</v>
       </c>
       <c r="B6">
-        <v>12.32192809</v>
+        <f t="shared" si="0"/>
+        <v>12.321928094887364</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>1.9500000000000028</v>
+        <f t="shared" si="1"/>
+        <v>0.67807190511263782</v>
       </c>
       <c r="D6">
-        <v>33.950000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.6</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6144</v>
       </c>
       <c r="B7">
-        <v>12.5849625</v>
+        <f t="shared" si="0"/>
+        <v>12.584962500721158</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>2.2100000000000009</v>
+        <f t="shared" si="1"/>
+        <v>1.028569152196771</v>
       </c>
       <c r="D7">
-        <v>34.21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.04</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7168</v>
       </c>
       <c r="B8">
-        <v>12.80735492</v>
+        <f t="shared" si="0"/>
+        <v>12.807354922057604</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>1.9299999999999997</v>
+        <f t="shared" si="1"/>
+        <v>1.028569152196771</v>
       </c>
       <c r="D8">
-        <v>33.93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.04</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8192</v>
       </c>
       <c r="B9">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>1.9699999999999989</v>
+        <f t="shared" si="1"/>
+        <v>1.0214797274104515</v>
       </c>
       <c r="D9">
-        <v>33.97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9216</v>
       </c>
       <c r="B10">
-        <v>13.169924999999999</v>
+        <f t="shared" si="0"/>
+        <v>13.169925001442312</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>2.0600000000000023</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>34.06</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10240</v>
       </c>
       <c r="B11">
-        <v>13.32192809</v>
+        <f t="shared" si="0"/>
+        <v>13.321928094887364</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>2.1499999999999986</v>
+        <f t="shared" si="1"/>
+        <v>0.98550043030488488</v>
       </c>
       <c r="D11">
-        <v>34.15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.98</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11264</v>
       </c>
       <c r="B12">
-        <v>13.45943162</v>
+        <f t="shared" si="0"/>
+        <v>13.459431618637296</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="D12">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12288</v>
       </c>
       <c r="B13">
-        <v>13.5849625</v>
+        <f t="shared" si="0"/>
+        <v>13.584962500721158</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
-        <v>2.2700000000000031</v>
+        <f t="shared" si="1"/>
+        <v>0.97085365434048343</v>
       </c>
       <c r="D13">
-        <v>34.270000000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.96</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13312</v>
       </c>
       <c r="B14">
-        <v>13.70043972</v>
+        <f t="shared" si="0"/>
+        <v>13.700439718141093</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>2.2899999999999991</v>
+        <f t="shared" si="1"/>
+        <v>1.0143552929770701</v>
       </c>
       <c r="D14">
-        <v>34.29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.02</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14336</v>
       </c>
       <c r="B15">
-        <v>13.80735492</v>
+        <f t="shared" si="0"/>
+        <v>13.807354922057604</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
-        <v>2.1199999999999974</v>
+        <f t="shared" si="1"/>
+        <v>1.0772429989324603</v>
       </c>
       <c r="D15">
-        <v>34.119999999999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.11</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15360</v>
       </c>
       <c r="B16">
-        <v>13.906890600000001</v>
+        <f t="shared" si="0"/>
+        <v>13.906890595608518</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
-        <v>2.1000000000000014</v>
+        <f t="shared" si="1"/>
+        <v>1.0496307677246004</v>
       </c>
       <c r="D16">
-        <v>34.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16384</v>
       </c>
       <c r="B17">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
-        <v>2.2299999999999969</v>
+        <f t="shared" si="1"/>
+        <v>1.0840642647884746</v>
       </c>
       <c r="D17">
-        <v>34.229999999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.12</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17408</v>
       </c>
       <c r="B18">
-        <v>14.087462840000001</v>
+        <f t="shared" si="0"/>
+        <v>14.087462841250341</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
-        <v>2.1599999999999966</v>
+        <f t="shared" si="1"/>
+        <v>0.97819562968165163</v>
       </c>
       <c r="D18">
-        <v>34.159999999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.97</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18432</v>
       </c>
       <c r="B19">
-        <v>14.169924999999999</v>
+        <f t="shared" si="0"/>
+        <v>14.169925001442312</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
-        <v>2.2199999999999989</v>
+        <f t="shared" si="1"/>
+        <v>0.94860084749335571</v>
       </c>
       <c r="D19">
-        <v>34.22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.93</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19456</v>
       </c>
       <c r="B20">
-        <v>14.24792751</v>
+        <f t="shared" si="0"/>
+        <v>14.247927513443587</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>2.009999999999998</v>
+        <f t="shared" si="1"/>
+        <v>0.90303827011291216</v>
       </c>
       <c r="D20">
-        <v>34.01</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.87</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20480</v>
       </c>
       <c r="B21">
-        <v>14.32192809</v>
+        <f t="shared" si="0"/>
+        <v>14.321928094887364</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
-        <v>2.2100000000000009</v>
+        <f t="shared" si="1"/>
+        <v>0.95605665241240301</v>
       </c>
       <c r="D21">
-        <v>34.21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.94</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21504</v>
       </c>
       <c r="B22">
-        <v>14.392317419999999</v>
+        <f t="shared" si="0"/>
+        <v>14.392317422778762</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
-        <v>2.0200000000000031</v>
+        <f t="shared" si="1"/>
+        <v>1.2203299548795556</v>
       </c>
       <c r="D22">
-        <v>34.020000000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.33</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22528</v>
       </c>
       <c r="B23">
-        <v>14.45943162</v>
+        <f t="shared" si="0"/>
+        <v>14.459431618637296</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
-        <v>1.9500000000000028</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>33.950000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23552</v>
       </c>
       <c r="B24">
-        <v>14.52356196</v>
+        <f t="shared" si="0"/>
+        <v>14.523561956057014</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
-        <v>2.1000000000000014</v>
+        <f t="shared" si="1"/>
+        <v>1.0214797274104515</v>
       </c>
       <c r="D24">
-        <v>34.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24576</v>
       </c>
       <c r="B25">
-        <v>14.5849625</v>
+        <f t="shared" si="0"/>
+        <v>14.584962500721158</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>0.97819562968165163</v>
       </c>
       <c r="D25">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.97</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25600</v>
       </c>
       <c r="B26">
-        <v>14.643856189999999</v>
+        <f t="shared" si="0"/>
+        <v>14.643856189774723</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
-        <v>1.8999999999999986</v>
+        <f t="shared" si="1"/>
+        <v>1.0565835283663676</v>
       </c>
       <c r="D26">
-        <v>33.9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.08</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26624</v>
       </c>
       <c r="B27">
-        <v>14.70043972</v>
+        <f t="shared" si="0"/>
+        <v>14.700439718141093</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
-        <v>2.0499999999999972</v>
+        <f t="shared" si="1"/>
+        <v>1.1243281350022019</v>
       </c>
       <c r="D27">
-        <v>34.049999999999997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27648</v>
       </c>
       <c r="B28">
-        <v>14.754887500000001</v>
+        <f t="shared" si="0"/>
+        <v>14.754887502163468</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
-        <v>2.1199999999999974</v>
+        <f t="shared" si="1"/>
+        <v>1.2630344058337937</v>
       </c>
       <c r="D28">
-        <v>34.119999999999997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.4</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28672</v>
       </c>
       <c r="B29">
-        <v>14.80735492</v>
+        <f t="shared" si="0"/>
+        <v>14.807354922057604</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
-        <v>2.2100000000000009</v>
+        <f t="shared" si="1"/>
+        <v>1.1440463696167069</v>
       </c>
       <c r="D29">
-        <v>34.21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.21</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29696</v>
       </c>
       <c r="B30">
-        <v>14.857981000000001</v>
+        <f t="shared" si="0"/>
+        <v>14.857980995127573</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
-        <v>3.2700000000000031</v>
+        <f t="shared" si="1"/>
+        <v>1.2203299548795556</v>
       </c>
       <c r="D30">
-        <v>35.270000000000003</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.33</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30720</v>
       </c>
       <c r="B31">
-        <v>14.906890600000001</v>
+        <f t="shared" si="0"/>
+        <v>14.906890595608518</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
-        <v>2.3999999999999986</v>
+        <f t="shared" si="1"/>
+        <v>1.3785116232537298</v>
       </c>
       <c r="D31">
-        <v>34.4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.6</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31744</v>
       </c>
       <c r="B32">
-        <v>14.95419631</v>
+        <f t="shared" si="0"/>
+        <v>14.954196310386875</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
-        <v>2.5600000000000023</v>
+        <f t="shared" si="1"/>
+        <v>1.7004397181410922</v>
       </c>
       <c r="D32">
-        <v>34.56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.25</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32768</v>
       </c>
       <c r="B33">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
-        <v>3.0799999999999983</v>
+        <f t="shared" si="1"/>
+        <v>2.6064422281316078</v>
       </c>
       <c r="D33">
-        <v>35.08</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6.09</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>33792</v>
+        <v>49152</v>
       </c>
       <c r="B34">
-        <v>15.04439412</v>
+        <f t="shared" si="0"/>
+        <v>15.584962500721158</v>
       </c>
       <c r="C34">
-        <f t="shared" si="0"/>
-        <v>5.6499999999999986</v>
+        <f t="shared" si="1"/>
+        <v>2.3074285251922473</v>
       </c>
       <c r="D34">
-        <v>37.65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4.95</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>34816</v>
+        <v>65536</v>
       </c>
       <c r="B35">
-        <v>15.087462840000001</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="C35">
-        <f t="shared" si="0"/>
-        <v>3.5300000000000011</v>
+        <f t="shared" si="1"/>
+        <v>2.304511041809953</v>
       </c>
       <c r="D35">
-        <v>35.53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>35840</v>
+        <v>81920</v>
       </c>
       <c r="B36">
-        <v>15.129283020000001</v>
+        <f t="shared" si="0"/>
+        <v>16.321928094887365</v>
       </c>
       <c r="C36">
-        <f t="shared" si="0"/>
-        <v>3.9099999999999966</v>
+        <f t="shared" si="1"/>
+        <v>1.9963887464476213</v>
       </c>
       <c r="D36">
-        <v>35.909999999999997</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.99</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>36864</v>
+        <v>98304</v>
       </c>
       <c r="B37">
-        <v>15.169924999999999</v>
+        <f t="shared" si="0"/>
+        <v>16.584962500721158</v>
       </c>
       <c r="C37">
-        <f t="shared" si="0"/>
-        <v>3.25</v>
+        <f t="shared" si="1"/>
+        <v>2.2986583155645151</v>
       </c>
       <c r="D37">
-        <v>35.25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4.92</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>37888</v>
+        <v>114688</v>
       </c>
       <c r="B38">
-        <v>15.20945337</v>
+        <f t="shared" si="0"/>
+        <v>16.807354922057606</v>
       </c>
       <c r="C38">
-        <f t="shared" si="0"/>
-        <v>4.0600000000000023</v>
+        <f t="shared" si="1"/>
+        <v>2.4302852729777809</v>
       </c>
       <c r="D38">
-        <v>36.06</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5.39</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>38912</v>
+        <v>131072</v>
       </c>
       <c r="B39">
-        <v>15.24792751</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="C39">
-        <f t="shared" si="0"/>
-        <v>3.5499999999999972</v>
+        <f t="shared" si="1"/>
+        <v>5.6458745503090304</v>
       </c>
       <c r="D39">
-        <v>35.549999999999997</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50.07</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>39936</v>
+        <v>196608</v>
       </c>
       <c r="B40">
-        <v>15.28540222</v>
+        <f t="shared" si="0"/>
+        <v>17.584962500721158</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
-        <v>4.3999999999999986</v>
+        <f t="shared" si="1"/>
+        <v>3.1667154449664223</v>
       </c>
       <c r="D40">
-        <v>36.4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8.98</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>40960</v>
+        <v>262144</v>
       </c>
       <c r="B41">
-        <v>15.32192809</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="C41">
-        <f t="shared" si="0"/>
-        <v>3.7199999999999989</v>
+        <f t="shared" si="1"/>
+        <v>4.0098845889318442</v>
       </c>
       <c r="D41">
-        <v>35.72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16.11</v>
+      </c>
+      <c r="E41">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>41984</v>
+        <v>327680</v>
       </c>
       <c r="B42">
-        <v>15.357552</v>
+        <f t="shared" si="0"/>
+        <v>18.321928094887365</v>
       </c>
       <c r="C42">
-        <f t="shared" si="0"/>
-        <v>4.6899999999999977</v>
+        <f t="shared" si="1"/>
+        <v>4.4685833170068276</v>
       </c>
       <c r="D42">
-        <v>36.69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>22.14</v>
+      </c>
+      <c r="E42">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>43008</v>
+        <v>393216</v>
       </c>
       <c r="B43">
-        <v>15.392317419999999</v>
+        <f t="shared" si="0"/>
+        <v>18.584962500721154</v>
       </c>
       <c r="C43">
-        <f t="shared" si="0"/>
-        <v>3.8599999999999994</v>
+        <f t="shared" si="1"/>
+        <v>4.4899282194051828</v>
       </c>
       <c r="D43">
-        <v>35.86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+        <v>22.47</v>
+      </c>
+      <c r="E43">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>44032</v>
+        <v>458752</v>
       </c>
       <c r="B44">
-        <v>15.42626475</v>
+        <f t="shared" si="0"/>
+        <v>18.807354922057606</v>
       </c>
       <c r="C44">
-        <f t="shared" si="0"/>
-        <v>4.0499999999999972</v>
+        <f t="shared" si="1"/>
+        <v>4.6229303509201767</v>
       </c>
       <c r="D44">
-        <v>36.049999999999997</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24.64</v>
+      </c>
+      <c r="E44">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>45056</v>
+        <v>524288</v>
       </c>
       <c r="B45">
-        <v>15.45943162</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="C45">
-        <f t="shared" si="0"/>
-        <v>4.7199999999999989</v>
+        <f t="shared" si="1"/>
+        <v>4.7554217347342425</v>
       </c>
       <c r="D45">
-        <v>36.72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27.01</v>
+      </c>
+      <c r="E45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>49152</v>
+        <v>1048576</v>
       </c>
       <c r="B46">
-        <v>15.5849625</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="C46">
-        <f t="shared" si="0"/>
-        <v>3.9799999999999969</v>
+        <f t="shared" si="1"/>
+        <v>7.0296737346264209</v>
       </c>
       <c r="D46">
-        <v>35.979999999999997</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>130.66</v>
+      </c>
+      <c r="E46">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>65536</v>
+        <v>2097152</v>
       </c>
       <c r="B47">
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="C47">
-        <f t="shared" si="0"/>
-        <v>4.8599999999999994</v>
+        <f t="shared" si="1"/>
+        <v>8.0635029423061582</v>
       </c>
       <c r="D47">
-        <v>36.86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+        <v>267.52</v>
+      </c>
+      <c r="E47">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>81920</v>
+        <v>3145728</v>
       </c>
       <c r="B48">
-        <v>16.32192809</v>
+        <f t="shared" si="0"/>
+        <v>21.584962500721154</v>
       </c>
       <c r="C48">
-        <f t="shared" si="0"/>
-        <v>4.0300000000000011</v>
+        <f t="shared" si="1"/>
+        <v>6.9971794809376213</v>
       </c>
       <c r="D48">
-        <v>36.03</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>127.75</v>
+      </c>
+      <c r="E48">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>98304</v>
+        <v>4194304</v>
       </c>
       <c r="B49">
-        <v>16.5849625</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="C49">
-        <f t="shared" si="0"/>
-        <v>71.77</v>
+        <f t="shared" si="1"/>
+        <v>7.5055734002820182</v>
       </c>
       <c r="D49">
-        <v>103.77</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>181.72</v>
+      </c>
+      <c r="E49">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>114688</v>
+        <v>5242880</v>
       </c>
       <c r="B50">
-        <v>16.807354920000002</v>
+        <f t="shared" si="0"/>
+        <v>22.321928094887362</v>
       </c>
       <c r="C50">
-        <f t="shared" si="0"/>
-        <v>6.9099999999999966</v>
+        <f t="shared" si="1"/>
+        <v>7.6603525096709211</v>
       </c>
       <c r="D50">
-        <v>38.909999999999997</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>202.3</v>
+      </c>
+      <c r="E50">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>131072</v>
+        <v>6291456</v>
       </c>
       <c r="B51">
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>22.584962500721158</v>
       </c>
       <c r="C51">
-        <f t="shared" si="0"/>
-        <v>4.0399999999999991</v>
+        <f t="shared" si="1"/>
+        <v>8.3048760500448893</v>
       </c>
       <c r="D51">
-        <v>36.04</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>316.24</v>
+      </c>
+      <c r="E51">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>147456</v>
+        <v>7340032</v>
       </c>
       <c r="B52">
-        <v>17.169924999999999</v>
+        <f t="shared" si="0"/>
+        <v>22.807354922057606</v>
       </c>
       <c r="C52">
-        <f t="shared" si="0"/>
-        <v>5.93</v>
+        <f t="shared" si="1"/>
+        <v>9.179088012680273</v>
       </c>
       <c r="D52">
-        <v>37.93</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>579.66999999999996</v>
+      </c>
+      <c r="E52">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>163840</v>
+        <v>8388608</v>
       </c>
       <c r="B53">
-        <v>17.32192809</v>
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
       <c r="C53">
-        <f t="shared" si="0"/>
-        <v>9.4799999999999969</v>
+        <f t="shared" si="1"/>
+        <v>7.8182626083044742</v>
       </c>
       <c r="D53">
-        <v>41.48</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>225.7</v>
+      </c>
+      <c r="E53">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>180224</v>
+        <v>9437184</v>
       </c>
       <c r="B54">
-        <v>17.45943162</v>
+        <f t="shared" si="0"/>
+        <v>23.169925001442316</v>
       </c>
       <c r="C54">
-        <f t="shared" si="0"/>
-        <v>7.8800000000000026</v>
+        <f t="shared" si="1"/>
+        <v>7.8026456041288244</v>
       </c>
       <c r="D54">
-        <v>39.880000000000003</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>223.27</v>
+      </c>
+      <c r="E54">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>196608</v>
+        <v>10485760</v>
       </c>
       <c r="B55">
-        <v>17.5849625</v>
+        <f t="shared" si="0"/>
+        <v>23.321928094887362</v>
       </c>
       <c r="C55">
-        <f t="shared" si="0"/>
-        <v>6.5200000000000031</v>
+        <f t="shared" si="1"/>
+        <v>7.7631459581494759</v>
       </c>
       <c r="D55">
-        <v>38.520000000000003</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>217.24</v>
+      </c>
+      <c r="E55">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>212992</v>
+        <v>11534336</v>
       </c>
       <c r="B56">
-        <v>17.700439719999999</v>
+        <f t="shared" si="0"/>
+        <v>23.459431618637296</v>
       </c>
       <c r="C56">
-        <f t="shared" si="0"/>
-        <v>8.7100000000000009</v>
+        <f t="shared" si="1"/>
+        <v>7.8880125854028291</v>
       </c>
       <c r="D56">
-        <v>40.71</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+        <v>236.88</v>
+      </c>
+      <c r="E56">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>229376</v>
+        <v>12582912</v>
       </c>
       <c r="B57">
-        <v>17.807354920000002</v>
+        <f t="shared" si="0"/>
+        <v>23.584962500721158</v>
       </c>
       <c r="C57">
-        <f t="shared" si="0"/>
-        <v>19.310000000000002</v>
+        <f t="shared" si="1"/>
+        <v>7.768184324776926</v>
       </c>
       <c r="D57">
-        <v>51.31</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+      <c r="E57">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>245760</v>
+        <v>13631488</v>
       </c>
       <c r="B58">
-        <v>17.906890600000001</v>
+        <f t="shared" si="0"/>
+        <v>23.700439718141094</v>
       </c>
       <c r="C58">
-        <f t="shared" si="0"/>
-        <v>18.009999999999998</v>
+        <f t="shared" si="1"/>
+        <v>7.7666614118172621</v>
       </c>
       <c r="D58">
-        <v>50.01</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>217.77</v>
+      </c>
+      <c r="E58">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>262144</v>
+        <v>14680064</v>
       </c>
       <c r="B59">
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>23.807354922057602</v>
       </c>
       <c r="C59">
-        <f t="shared" si="0"/>
-        <v>16.659999999999997</v>
+        <f t="shared" si="1"/>
+        <v>8.0164183174068757</v>
       </c>
       <c r="D59">
-        <v>48.66</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>258.93</v>
+      </c>
+      <c r="E59">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>278528</v>
+        <v>15728640</v>
       </c>
       <c r="B60">
-        <v>18.087462840000001</v>
+        <f t="shared" si="0"/>
+        <v>23.906890595608516</v>
       </c>
       <c r="C60">
-        <f t="shared" si="0"/>
-        <v>16.759999999999998</v>
+        <f t="shared" si="1"/>
+        <v>7.7781428544637716</v>
       </c>
       <c r="D60">
-        <v>48.76</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>219.51</v>
+      </c>
+      <c r="E60">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>294912</v>
+        <v>16777216</v>
       </c>
       <c r="B61">
-        <v>18.169924999999999</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="C61">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>8.0241977648948684</v>
       </c>
       <c r="D61">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+        <v>260.33</v>
+      </c>
+      <c r="E61">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>311296</v>
+        <v>17825792</v>
       </c>
       <c r="B62">
-        <v>18.24792751</v>
+        <f t="shared" si="0"/>
+        <v>24.087462841250343</v>
       </c>
       <c r="C62">
-        <f t="shared" si="0"/>
-        <v>22.619999999999997</v>
+        <f t="shared" si="1"/>
+        <v>7.8578566195043322</v>
       </c>
       <c r="D62">
-        <v>54.62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+        <v>231.98</v>
+      </c>
+      <c r="E62">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>327680</v>
+        <v>18874368</v>
       </c>
       <c r="B63">
-        <v>18.32192809</v>
+        <f t="shared" si="0"/>
+        <v>24.169925001442312</v>
       </c>
       <c r="C63">
-        <f t="shared" si="0"/>
-        <v>89.36</v>
+        <f t="shared" si="1"/>
+        <v>7.8548683832602366</v>
       </c>
       <c r="D63">
-        <v>121.36</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+        <v>231.5</v>
+      </c>
+      <c r="E63">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>344064</v>
+        <v>19922944</v>
       </c>
       <c r="B64">
-        <v>18.392317420000001</v>
+        <f t="shared" si="0"/>
+        <v>24.247927513443585</v>
       </c>
       <c r="C64">
-        <f t="shared" si="0"/>
-        <v>21.840000000000003</v>
+        <f t="shared" si="1"/>
+        <v>8.0350739973776228</v>
       </c>
       <c r="D64">
-        <v>53.84</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+        <v>262.3</v>
+      </c>
+      <c r="E64">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>360448</v>
+        <v>20971520</v>
       </c>
       <c r="B65">
-        <v>18.45943162</v>
+        <f t="shared" si="0"/>
+        <v>24.321928094887365</v>
       </c>
       <c r="C65">
-        <f t="shared" si="0"/>
-        <v>22.42</v>
+        <f t="shared" si="1"/>
+        <v>8.2035437752826574</v>
       </c>
       <c r="D65">
-        <v>54.42</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+        <v>294.79000000000002</v>
+      </c>
+      <c r="E65">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>376832</v>
+        <v>22020096</v>
       </c>
       <c r="B66">
-        <v>18.523561959999999</v>
+        <f t="shared" si="0"/>
+        <v>24.392317422778763</v>
       </c>
       <c r="C66">
-        <f t="shared" si="0"/>
-        <v>23.67</v>
+        <f t="shared" si="1"/>
+        <v>7.898389766534847</v>
       </c>
       <c r="D66">
-        <v>55.67</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+        <v>238.59</v>
+      </c>
+      <c r="E66">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>393216</v>
+        <v>23068672</v>
       </c>
       <c r="B67">
-        <v>18.5849625</v>
+        <f t="shared" ref="B67:B70" si="2">LOG(A67,2)</f>
+        <v>24.459431618637296</v>
       </c>
       <c r="C67">
-        <f t="shared" si="0"/>
-        <v>24.93</v>
+        <f t="shared" ref="C67:C70" si="3">LOG(D67,2)</f>
+        <v>7.9302050977844338</v>
       </c>
       <c r="D67">
-        <v>56.93</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+        <v>243.91</v>
+      </c>
+      <c r="E67">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>409600</v>
+        <v>24117248</v>
       </c>
       <c r="B68">
-        <v>18.643856190000001</v>
+        <f t="shared" si="2"/>
+        <v>24.523561956057016</v>
       </c>
       <c r="C68">
-        <f t="shared" si="0"/>
-        <v>22.689999999999998</v>
+        <f t="shared" si="3"/>
+        <v>8.2011437320530334</v>
       </c>
       <c r="D68">
-        <v>54.69</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+        <v>294.3</v>
+      </c>
+      <c r="E68">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>425984</v>
+        <v>25165824</v>
       </c>
       <c r="B69">
-        <v>18.700439719999999</v>
+        <f t="shared" si="2"/>
+        <v>24.584962500721158</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69:C108" si="1">D69-32</f>
-        <v>37.480000000000004</v>
+        <f t="shared" si="3"/>
+        <v>7.9467893339488453</v>
       </c>
       <c r="D69">
-        <v>69.48</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+        <v>246.73</v>
+      </c>
+      <c r="E69">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>442368</v>
+        <v>26214400</v>
       </c>
       <c r="B70">
-        <v>18.754887499999999</v>
+        <f t="shared" si="2"/>
+        <v>24.643856189774727</v>
       </c>
       <c r="C70">
-        <f t="shared" si="1"/>
-        <v>23.32</v>
+        <f t="shared" si="3"/>
+        <v>7.8644337963656232</v>
       </c>
       <c r="D70">
-        <v>55.32</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>458752</v>
-      </c>
-      <c r="B71">
-        <v>18.807354920000002</v>
-      </c>
-      <c r="C71">
-        <f t="shared" si="1"/>
-        <v>24.880000000000003</v>
-      </c>
-      <c r="D71">
-        <v>56.88</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>475136</v>
-      </c>
-      <c r="B72">
-        <v>18.857980999999999</v>
-      </c>
-      <c r="C72">
-        <f t="shared" si="1"/>
-        <v>119.68</v>
-      </c>
-      <c r="D72">
-        <v>151.68</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>491520</v>
-      </c>
-      <c r="B73">
-        <v>18.906890600000001</v>
-      </c>
-      <c r="C73">
-        <f t="shared" si="1"/>
-        <v>26.14</v>
-      </c>
-      <c r="D73">
-        <v>58.14</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>507904</v>
-      </c>
-      <c r="B74">
-        <v>18.95419631</v>
-      </c>
-      <c r="C74">
-        <f t="shared" si="1"/>
-        <v>93.72</v>
-      </c>
-      <c r="D74">
-        <v>125.72</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>524288</v>
-      </c>
-      <c r="B75">
-        <v>19</v>
-      </c>
-      <c r="C75">
-        <f t="shared" si="1"/>
-        <v>26.71</v>
-      </c>
-      <c r="D75">
-        <v>58.71</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>1048576</v>
-      </c>
-      <c r="B76">
-        <v>20</v>
-      </c>
-      <c r="C76">
-        <f t="shared" si="1"/>
-        <v>44.08</v>
-      </c>
-      <c r="D76">
-        <v>76.08</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>2097152</v>
-      </c>
-      <c r="B77">
-        <v>21</v>
-      </c>
-      <c r="C77">
-        <f t="shared" si="1"/>
-        <v>183.84</v>
-      </c>
-      <c r="D77">
-        <v>215.84</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>3145728</v>
-      </c>
-      <c r="B78">
-        <v>21.5849625</v>
-      </c>
-      <c r="C78">
-        <f t="shared" si="1"/>
-        <v>254.85000000000002</v>
-      </c>
-      <c r="D78">
-        <v>286.85000000000002</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>4194304</v>
-      </c>
-      <c r="B79">
-        <v>22</v>
-      </c>
-      <c r="C79">
-        <f t="shared" si="1"/>
-        <v>278.93</v>
-      </c>
-      <c r="D79">
-        <v>310.93</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>5242880</v>
-      </c>
-      <c r="B80">
-        <v>22.32192809</v>
-      </c>
-      <c r="C80">
-        <f t="shared" si="1"/>
-        <v>488.15</v>
-      </c>
-      <c r="D80">
-        <v>520.15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>6291456</v>
-      </c>
-      <c r="B81">
-        <v>22.5849625</v>
-      </c>
-      <c r="C81">
-        <f t="shared" si="1"/>
-        <v>322.64</v>
-      </c>
-      <c r="D81">
-        <v>354.64</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>7340032</v>
-      </c>
-      <c r="B82">
-        <v>22.807354920000002</v>
-      </c>
-      <c r="C82">
-        <f t="shared" si="1"/>
-        <v>208.99</v>
-      </c>
-      <c r="D82">
-        <v>240.99</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>8388608</v>
-      </c>
-      <c r="B83">
-        <v>23</v>
-      </c>
-      <c r="C83">
-        <f t="shared" si="1"/>
-        <v>311.70999999999998</v>
-      </c>
-      <c r="D83">
-        <v>343.71</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>9437184</v>
-      </c>
-      <c r="B84">
-        <v>23.169924999999999</v>
-      </c>
-      <c r="C84">
-        <f t="shared" si="1"/>
-        <v>327.08999999999997</v>
-      </c>
-      <c r="D84">
-        <v>359.09</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>10485760</v>
-      </c>
-      <c r="B85">
-        <v>23.32192809</v>
-      </c>
-      <c r="C85">
-        <f t="shared" si="1"/>
-        <v>310.02999999999997</v>
-      </c>
-      <c r="D85">
-        <v>342.03</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>11534336</v>
-      </c>
-      <c r="B86">
-        <v>23.45943162</v>
-      </c>
-      <c r="C86">
-        <f t="shared" si="1"/>
-        <v>226.83999999999997</v>
-      </c>
-      <c r="D86">
-        <v>258.83999999999997</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>12582912</v>
-      </c>
-      <c r="B87">
-        <v>23.5849625</v>
-      </c>
-      <c r="C87">
-        <f t="shared" si="1"/>
-        <v>271.01</v>
-      </c>
-      <c r="D87">
-        <v>303.01</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>13631488</v>
-      </c>
-      <c r="B88">
-        <v>23.700439719999999</v>
-      </c>
-      <c r="C88">
-        <f t="shared" si="1"/>
-        <v>297.89</v>
-      </c>
-      <c r="D88">
-        <v>329.89</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>14680064</v>
-      </c>
-      <c r="B89">
-        <v>23.807354920000002</v>
-      </c>
-      <c r="C89">
-        <f t="shared" si="1"/>
-        <v>430.9</v>
-      </c>
-      <c r="D89">
-        <v>462.9</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>15728640</v>
-      </c>
-      <c r="B90">
-        <v>23.906890600000001</v>
-      </c>
-      <c r="C90">
-        <f t="shared" si="1"/>
-        <v>293.38</v>
-      </c>
-      <c r="D90">
-        <v>325.38</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>16777216</v>
-      </c>
-      <c r="B91">
-        <v>24</v>
-      </c>
-      <c r="C91">
-        <f t="shared" si="1"/>
-        <v>251.33999999999997</v>
-      </c>
-      <c r="D91">
-        <v>283.33999999999997</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>17825792</v>
-      </c>
-      <c r="B92">
-        <v>24.087462840000001</v>
-      </c>
-      <c r="C92">
-        <f t="shared" si="1"/>
-        <v>231.98000000000002</v>
-      </c>
-      <c r="D92">
-        <v>263.98</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>18874368</v>
-      </c>
-      <c r="B93">
-        <v>24.169924999999999</v>
-      </c>
-      <c r="C93">
-        <f t="shared" si="1"/>
-        <v>378.18</v>
-      </c>
-      <c r="D93">
-        <v>410.18</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>19922944</v>
-      </c>
-      <c r="B94">
-        <v>24.24792751</v>
-      </c>
-      <c r="C94">
-        <f t="shared" si="1"/>
-        <v>263.45999999999998</v>
-      </c>
-      <c r="D94">
-        <v>295.45999999999998</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>20971520</v>
-      </c>
-      <c r="B95">
-        <v>24.32192809</v>
-      </c>
-      <c r="C95">
-        <f t="shared" si="1"/>
-        <v>356.44</v>
-      </c>
-      <c r="D95">
-        <v>388.44</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>22020096</v>
-      </c>
-      <c r="B96">
-        <v>24.392317420000001</v>
-      </c>
-      <c r="C96">
-        <f t="shared" si="1"/>
-        <v>347.18</v>
-      </c>
-      <c r="D96">
-        <v>379.18</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>23068672</v>
-      </c>
-      <c r="B97">
-        <v>24.45943162</v>
-      </c>
-      <c r="C97">
-        <f t="shared" si="1"/>
-        <v>265.14999999999998</v>
-      </c>
-      <c r="D97">
-        <v>297.14999999999998</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>24117248</v>
-      </c>
-      <c r="B98">
-        <v>24.523561959999999</v>
-      </c>
-      <c r="C98">
-        <f t="shared" si="1"/>
-        <v>290.75</v>
-      </c>
-      <c r="D98">
-        <v>322.75</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>25165824</v>
-      </c>
-      <c r="B99">
-        <v>24.5849625</v>
-      </c>
-      <c r="C99">
-        <f t="shared" si="1"/>
-        <v>295.98</v>
-      </c>
-      <c r="D99">
-        <v>327.98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>26214400</v>
-      </c>
-      <c r="B100">
-        <v>24.643856190000001</v>
-      </c>
-      <c r="C100">
-        <f t="shared" si="1"/>
-        <v>306.08999999999997</v>
-      </c>
-      <c r="D100">
-        <v>338.09</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>27262976</v>
-      </c>
-      <c r="B101">
-        <v>24.700439719999999</v>
-      </c>
-      <c r="C101">
-        <f t="shared" si="1"/>
-        <v>335.35</v>
-      </c>
-      <c r="D101">
-        <v>367.35</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102">
-        <v>28311552</v>
-      </c>
-      <c r="B102">
-        <v>24.754887499999999</v>
-      </c>
-      <c r="C102">
-        <f t="shared" si="1"/>
-        <v>270.88</v>
-      </c>
-      <c r="D102">
-        <v>302.88</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103">
-        <v>29360128</v>
-      </c>
-      <c r="B103">
-        <v>24.807354920000002</v>
-      </c>
-      <c r="C103">
-        <f t="shared" si="1"/>
-        <v>268.95999999999998</v>
-      </c>
-      <c r="D103">
-        <v>300.95999999999998</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104">
-        <v>30408704</v>
-      </c>
-      <c r="B104">
-        <v>24.857980999999999</v>
-      </c>
-      <c r="C104">
-        <f t="shared" si="1"/>
-        <v>302.52</v>
-      </c>
-      <c r="D104">
-        <v>334.52</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105">
-        <v>31457280</v>
-      </c>
-      <c r="B105">
-        <v>24.906890600000001</v>
-      </c>
-      <c r="C105">
-        <f t="shared" si="1"/>
-        <v>260.66000000000003</v>
-      </c>
-      <c r="D105">
-        <v>292.66000000000003</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106">
-        <v>32505856</v>
-      </c>
-      <c r="B106">
-        <v>24.95419631</v>
-      </c>
-      <c r="C106">
-        <f t="shared" si="1"/>
-        <v>270.89999999999998</v>
-      </c>
-      <c r="D106">
-        <v>302.89999999999998</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107">
-        <v>33554432</v>
-      </c>
-      <c r="B107">
-        <v>25</v>
-      </c>
-      <c r="C107">
-        <f t="shared" si="1"/>
-        <v>273.26</v>
-      </c>
-      <c r="D107">
-        <v>305.26</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108">
-        <v>67108864</v>
-      </c>
-      <c r="B108">
-        <v>26</v>
-      </c>
-      <c r="C108">
-        <f t="shared" si="1"/>
-        <v>294.10000000000002</v>
-      </c>
-      <c r="D108">
-        <v>326.10000000000002</v>
+        <v>233.04</v>
+      </c>
+      <c r="E70">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>